<commit_message>
first 4 samples done
</commit_message>
<xml_diff>
--- a/Transplants_Sym_D_Counts.xlsx
+++ b/Transplants_Sym_D_Counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayrlindsay/Desktop/GITHUB/TLPR21/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F7FC72-08F2-7A43-8144-C530E885CCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48277AE1-1217-234A-8DC1-28EF9419CA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="500" windowWidth="16580" windowHeight="14240" xr2:uid="{B3B410EB-7B18-8948-AE1E-8D2AB3226EE9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24040" windowHeight="14240" xr2:uid="{B3B410EB-7B18-8948-AE1E-8D2AB3226EE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="157">
   <si>
     <t>Squares_Counted</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>Sym_Count_Date</t>
+  </si>
+  <si>
+    <t>This one was pretty weird, full of debris and super diluted</t>
   </si>
 </sst>
 </file>
@@ -897,17 +900,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893FF5F1-8187-5D4A-AA3A-F52C7ABDE372}">
-  <dimension ref="A1:T286"/>
+  <dimension ref="A1:U286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U152" sqref="U152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -5194,15 +5198,15 @@
         <v>31</v>
       </c>
       <c r="R129" t="e">
-        <f t="shared" ref="R129:R134" si="26">AVERAGE(J129:Q129)/I129</f>
+        <f t="shared" ref="R129:R133" si="26">AVERAGE(J129:Q129)/I129</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S129" t="e">
-        <f t="shared" ref="S129:S134" si="27">STDEV(J129:Q129)/I129</f>
+        <f t="shared" ref="S129:S133" si="27">STDEV(J129:Q129)/I129</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T129" t="e">
-        <f t="shared" ref="T129:T134" si="28">S129/R129*100</f>
+        <f t="shared" ref="T129:T133" si="28">S129/R129*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5701,7 +5705,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SP_EV</v>
@@ -5734,7 +5738,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SP_JQ1</v>
@@ -5767,7 +5771,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_0AZ4</v>
@@ -5800,7 +5804,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_0DW46</v>
@@ -5833,7 +5837,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_0EV1</v>
@@ -5866,7 +5870,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_0EV3</v>
@@ -5899,7 +5903,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_1AZ5</v>
@@ -5919,20 +5923,56 @@
       <c r="F151" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R151" t="e">
+      <c r="G151" s="1">
+        <v>44706</v>
+      </c>
+      <c r="H151" t="s">
+        <v>13</v>
+      </c>
+      <c r="I151">
+        <v>4</v>
+      </c>
+      <c r="J151">
+        <v>30</v>
+      </c>
+      <c r="K151">
+        <v>48</v>
+      </c>
+      <c r="L151">
+        <v>35</v>
+      </c>
+      <c r="M151">
+        <v>34</v>
+      </c>
+      <c r="N151">
+        <v>33</v>
+      </c>
+      <c r="O151">
+        <v>39</v>
+      </c>
+      <c r="P151">
+        <v>36</v>
+      </c>
+      <c r="Q151">
+        <v>30</v>
+      </c>
+      <c r="R151">
         <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S151" t="e">
+        <v>8.90625</v>
+      </c>
+      <c r="S151">
         <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T151" t="e">
+        <v>1.4573551140924537</v>
+      </c>
+      <c r="T151">
         <f t="shared" si="32"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
+        <v>16.36328549156439</v>
+      </c>
+      <c r="U151" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="152" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2AZ2</v>
@@ -5965,7 +6005,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2AZ21</v>
@@ -5998,7 +6038,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2AZ3</v>
@@ -6031,7 +6071,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2AZ7</v>
@@ -6064,7 +6104,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2AZ7</v>
@@ -6097,7 +6137,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2DW40</v>
@@ -6130,7 +6170,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2DW44</v>
@@ -6163,7 +6203,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2EV10</v>
@@ -6196,7 +6236,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="str">
         <f t="shared" si="29"/>
         <v>OFAV_SS_2EV3</v>
@@ -6909,17 +6949,47 @@
       <c r="F181" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R181" t="e">
+      <c r="G181" s="1">
+        <v>44706</v>
+      </c>
+      <c r="H181" t="s">
+        <v>13</v>
+      </c>
+      <c r="I181">
+        <v>3</v>
+      </c>
+      <c r="J181">
+        <v>107</v>
+      </c>
+      <c r="K181">
+        <v>132</v>
+      </c>
+      <c r="L181">
+        <v>121</v>
+      </c>
+      <c r="M181">
+        <v>113</v>
+      </c>
+      <c r="N181">
+        <v>145</v>
+      </c>
+      <c r="O181">
+        <v>98</v>
+      </c>
+      <c r="P181">
+        <v>114</v>
+      </c>
+      <c r="R181">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S181" t="e">
+        <v>39.523809523809526</v>
+      </c>
+      <c r="S181">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T181" t="e">
+        <v>5.2594082995500298</v>
+      </c>
+      <c r="T181">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>13.306936661512122</v>
       </c>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.2">
@@ -7008,17 +7078,44 @@
       <c r="F184" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="R184" t="e">
+      <c r="G184" s="1">
+        <v>44706</v>
+      </c>
+      <c r="H184" t="s">
+        <v>13</v>
+      </c>
+      <c r="I184">
+        <v>3</v>
+      </c>
+      <c r="J184">
+        <v>117</v>
+      </c>
+      <c r="K184">
+        <v>131</v>
+      </c>
+      <c r="L184">
+        <v>139</v>
+      </c>
+      <c r="M184">
+        <v>156</v>
+      </c>
+      <c r="N184">
+        <v>137</v>
+      </c>
+      <c r="O184">
+        <v>131</v>
+      </c>
+      <c r="R184">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S184" t="e">
+        <v>45.05555555555555</v>
+      </c>
+      <c r="S184">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T184" t="e">
+        <v>4.2604990144174257</v>
+      </c>
+      <c r="T184">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>9.4561013883494045</v>
       </c>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.2">
@@ -7107,17 +7204,44 @@
       <c r="F187" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="R187" t="e">
+      <c r="G187" s="1">
+        <v>44706</v>
+      </c>
+      <c r="H187" t="s">
+        <v>13</v>
+      </c>
+      <c r="I187">
+        <v>3</v>
+      </c>
+      <c r="J187">
+        <v>103</v>
+      </c>
+      <c r="K187">
+        <v>122</v>
+      </c>
+      <c r="L187">
+        <v>121</v>
+      </c>
+      <c r="M187">
+        <v>108</v>
+      </c>
+      <c r="N187">
+        <v>127</v>
+      </c>
+      <c r="O187">
+        <v>122</v>
+      </c>
+      <c r="R187">
         <f t="shared" si="33"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S187" t="e">
+        <v>39.055555555555557</v>
+      </c>
+      <c r="S187">
         <f t="shared" si="34"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T187" t="e">
+        <v>3.1369954958113571</v>
+      </c>
+      <c r="T187">
         <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
+        <v>8.0321364046378978</v>
       </c>
     </row>
     <row r="188" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>